<commit_message>
01 Helloworld.html 作成 (#1)
</commit_message>
<xml_diff>
--- a/プログラム作成履歴.xlsx
+++ b/プログラム作成履歴.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -36,9 +36,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>01HelloWorld.html</t>
+  </si>
+  <si>
     <t>概要</t>
     <rPh sb="0" eb="2">
       <t>ガイヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>console.logにHelloWorldを出力</t>
+    <rPh sb="23" eb="25">
+      <t>シュツリョク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -406,7 +416,7 @@
   <dimension ref="A1:D255"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -427,16 +437,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="2">
+        <v>43435</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1">

</xml_diff>

<commit_message>
15 add program history
</commit_message>
<xml_diff>
--- a/プログラム作成履歴.xlsx
+++ b/プログラム作成履歴.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -245,6 +245,13 @@
     <t>サイコロを作成</t>
     <rPh sb="5" eb="7">
       <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>npm run eslinｔ設定用にnpm install</t>
+    <rPh sb="14" eb="17">
+      <t>セッテイヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -612,7 +619,7 @@
   <dimension ref="A1:D267"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -926,9 +933,13 @@
       <c r="A28" s="1">
         <v>15</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="2">
+        <v>43458</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1">

</xml_diff>

<commit_message>
15 add npm eslint (#20)
* 15 git test branch

*  15 add text

* 15 add npm run eslint

* 15 add program history
</commit_message>
<xml_diff>
--- a/プログラム作成履歴.xlsx
+++ b/プログラム作成履歴.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -245,6 +245,13 @@
     <t>サイコロを作成</t>
     <rPh sb="5" eb="7">
       <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>npm run eslinｔ設定用にnpm install</t>
+    <rPh sb="14" eb="17">
+      <t>セッテイヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -612,7 +619,7 @@
   <dimension ref="A1:D267"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -926,9 +933,13 @@
       <c r="A28" s="1">
         <v>15</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="2">
+        <v>43458</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1">

</xml_diff>